<commit_message>
rename preconditions to contracts
</commit_message>
<xml_diff>
--- a/Results/Pilot-study-result.xlsx
+++ b/Results/Pilot-study-result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poojarani/gitProjects/CommentAnalysisInPharo/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C04505B-202D-0546-8089-953705ED5D63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26BF997-7AAE-AC4B-8504-D3CC65C48597}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>Observations</t>
-  </si>
-  <si>
-    <t>Precondition</t>
   </si>
   <si>
     <t>Dependnecy</t>
@@ -2944,6 +2941,9 @@
   <si>
     <t xml:space="preserve"> Instance Variables
  token: &lt;String&gt;</t>
+  </si>
+  <si>
+    <t>Contracts</t>
   </si>
 </sst>
 </file>
@@ -3433,9 +3433,9 @@
   </sheetPr>
   <dimension ref="A1:AE923"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3546,13 +3546,13 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="AC1" s="5"/>
       <c r="AD1" s="5"/>
@@ -3560,59 +3560,59 @@
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="11" t="s">
+        <v>651</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="J2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>653</v>
-      </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="O2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="R2" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="S2" s="11"/>
       <c r="T2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U2" s="11"/>
       <c r="V2" s="11"/>
@@ -3625,33 +3625,33 @@
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>46</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
       <c r="F3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="N3" s="10"/>
       <c r="O3" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
@@ -3669,33 +3669,33 @@
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="22" t="s">
         <v>53</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>54</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="J4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="M4" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="N4" s="10"/>
       <c r="O4" s="11"/>
@@ -3704,11 +3704,11 @@
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
       <c r="T4" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U4" s="6"/>
       <c r="V4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
@@ -3719,39 +3719,39 @@
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="E5" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="F5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
@@ -3760,7 +3760,7 @@
       <c r="T5" s="11"/>
       <c r="U5" s="6"/>
       <c r="V5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
@@ -3771,42 +3771,42 @@
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="F6" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="19" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K6" s="10"/>
       <c r="L6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="N6" s="11" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
@@ -3815,7 +3815,7 @@
       <c r="T6" s="11"/>
       <c r="U6" s="6"/>
       <c r="V6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
@@ -3826,31 +3826,31 @@
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>82</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
       <c r="F7" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
@@ -3868,47 +3868,47 @@
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="E8" s="22" t="s">
         <v>87</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>88</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="K8" s="10"/>
       <c r="M8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="N8" s="10" t="s">
-        <v>92</v>
-      </c>
       <c r="O8" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S8" s="11"/>
       <c r="T8" s="11"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
@@ -3919,13 +3919,13 @@
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -3937,7 +3937,7 @@
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
       <c r="T9" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
@@ -3947,26 +3947,26 @@
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
       <c r="AB9" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>101</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H10" s="11"/>
       <c r="J10" s="11"/>
@@ -3976,13 +3976,13 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W10" s="11"/>
       <c r="X10" s="11"/>
@@ -3993,56 +3993,56 @@
     </row>
     <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="15" t="s">
+        <v>656</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>657</v>
-      </c>
-      <c r="D11" s="22" t="s">
+      <c r="E11" s="22" t="s">
         <v>108</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>109</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="I11" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="K11" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="L11" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="M11" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>116</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
@@ -4053,45 +4053,45 @@
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="D12" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>121</v>
-      </c>
       <c r="E12" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="I12" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="J12" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="M12" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="N12" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="N12" s="10" t="s">
-        <v>128</v>
-      </c>
       <c r="O12" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
@@ -4103,40 +4103,40 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z12" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="Z12" s="6" t="s">
-        <v>130</v>
       </c>
       <c r="AA12" s="11"/>
       <c r="AB12" s="11"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="15" t="s">
         <v>132</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>133</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="L13" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="L13" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="M13" s="6"/>
       <c r="O13" s="11"/>
@@ -4154,45 +4154,45 @@
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="E14" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="F14" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="H14" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="I14" s="10" t="s">
         <v>145</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>146</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="M14" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="N14" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="N14" s="10" t="s">
-        <v>149</v>
-      </c>
       <c r="O14" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
@@ -4210,46 +4210,46 @@
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="E15" s="22" t="s">
         <v>153</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>154</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="M15" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="O15" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
       <c r="U15" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="V15" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="V15" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
@@ -4260,50 +4260,50 @@
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="D16" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="E16" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="F16" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="G16" s="11"/>
       <c r="H16" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="M16" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="N16" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="N16" s="10" t="s">
-        <v>171</v>
-      </c>
       <c r="O16" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="S16" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="S16" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="T16" s="11"/>
       <c r="U16" s="11"/>
@@ -4317,29 +4317,29 @@
     </row>
     <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="15" t="s">
         <v>175</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>176</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J17" s="11"/>
       <c r="M17" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
@@ -4355,120 +4355,120 @@
     </row>
     <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="D18" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="E18" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="F18" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="H18" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>187</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="L18" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="M18" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="N18" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="N18" s="10" t="s">
-        <v>192</v>
-      </c>
       <c r="O18" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="S18" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="S18" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="T18" s="11"/>
       <c r="U18" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="V18" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="V18" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z18" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="Z18" s="6" t="s">
-        <v>198</v>
       </c>
       <c r="AA18" s="11"/>
       <c r="AB18" s="11"/>
     </row>
     <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="D19" s="22" t="s">
         <v>201</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>202</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="L19" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="M19" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="L19" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="M19" s="6" t="s">
+      <c r="N19" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="N19" s="10" t="s">
-        <v>207</v>
-      </c>
       <c r="O19" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
       <c r="U19" s="11"/>
       <c r="V19" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="W19" s="11"/>
       <c r="X19" s="11"/>
@@ -4479,93 +4479,93 @@
     </row>
     <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="E20" s="22" t="s">
         <v>212</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>213</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>214</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>215</v>
       </c>
       <c r="J20" s="11"/>
       <c r="K20" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="M20" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="M20" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="N20" s="10"/>
       <c r="O20" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S20" s="11"/>
       <c r="T20" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U20" s="11"/>
       <c r="V20" s="11"/>
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Z20" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA20" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="AA20" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="AB20" s="11"/>
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="D21" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="E21" s="22" t="s">
         <v>226</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>227</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="I21" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="J21" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="K21" s="10" t="s">
         <v>230</v>
-      </c>
-      <c r="K21" s="10" t="s">
-        <v>231</v>
       </c>
       <c r="L21" s="10"/>
       <c r="M21" s="11"/>
@@ -4584,44 +4584,44 @@
     </row>
     <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="D22" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="E22" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="F22" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="G22" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="H22" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="I22" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="J22" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="L22" s="10" t="s">
         <v>241</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>242</v>
       </c>
       <c r="M22" s="11"/>
       <c r="O22" s="11"/>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
@@ -4658,7 +4658,7 @@
     </row>
     <row r="24" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="22"/>
@@ -4682,24 +4682,24 @@
     </row>
     <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>245</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>246</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J25" s="11"/>
       <c r="K25" s="10"/>
@@ -4709,7 +4709,7 @@
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="S25" s="11"/>
       <c r="T25" s="11"/>
@@ -4724,28 +4724,28 @@
     </row>
     <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="D26" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="E26" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="F26" s="6" t="s">
         <v>252</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>253</v>
       </c>
       <c r="G26" s="11"/>
       <c r="J26" s="11"/>
       <c r="K26" s="10"/>
       <c r="L26" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M26" s="11"/>
       <c r="N26" s="10"/>
@@ -4753,7 +4753,7 @@
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
       <c r="R26" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S26" s="11"/>
       <c r="T26" s="11"/>
@@ -4768,16 +4768,16 @@
     </row>
     <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="D27" s="22" t="s">
         <v>258</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>259</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="11"/>
@@ -4790,7 +4790,7 @@
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
       <c r="R27" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="S27" s="11"/>
       <c r="T27" s="11"/>
@@ -4805,19 +4805,19 @@
     </row>
     <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C28" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="C28" s="15" t="s">
+      <c r="D28" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="D28" s="22" t="s">
-        <v>263</v>
-      </c>
       <c r="E28" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -4833,44 +4833,44 @@
       <c r="T28" s="11"/>
       <c r="U28" s="6"/>
       <c r="V28" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="W28" s="11"/>
       <c r="X28" s="11"/>
       <c r="Y28" s="11"/>
       <c r="Z28" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="AA28" s="6" t="s">
         <v>265</v>
-      </c>
-      <c r="AA28" s="6" t="s">
-        <v>266</v>
       </c>
       <c r="AB28" s="6"/>
     </row>
     <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="D29" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="E29" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>271</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="19" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="J29" s="11"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M29" s="11"/>
       <c r="N29" s="10"/>
@@ -4878,7 +4878,7 @@
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
       <c r="R29" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="S29" s="11"/>
       <c r="T29" s="11"/>
@@ -4893,26 +4893,26 @@
     </row>
     <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="D30" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="E30" s="22" t="s">
         <v>277</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>278</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J30" s="11"/>
       <c r="K30" s="10"/>
@@ -4923,7 +4923,7 @@
       <c r="P30" s="10"/>
       <c r="Q30" s="10"/>
       <c r="R30" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="S30" s="11"/>
       <c r="T30" s="11"/>
@@ -4934,38 +4934,38 @@
       <c r="Y30" s="6"/>
       <c r="Z30" s="11"/>
       <c r="AA30" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AB30" s="6"/>
     </row>
     <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="C31" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="D31" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="E31" s="22" t="s">
         <v>284</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>285</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
       <c r="J31" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K31" s="10"/>
       <c r="M31" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N31" s="10"/>
       <c r="O31" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
@@ -4984,28 +4984,28 @@
     <row r="32" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="11"/>
       <c r="B32" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C32" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="D32" s="22" t="s">
         <v>289</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>290</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="11"/>
       <c r="G32" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="I32" s="10" t="s">
         <v>291</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>292</v>
       </c>
       <c r="J32" s="11"/>
       <c r="K32" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="L32" s="10" t="s">
         <v>293</v>
-      </c>
-      <c r="L32" s="10" t="s">
-        <v>294</v>
       </c>
       <c r="M32" s="11"/>
       <c r="N32" s="10"/>
@@ -5026,19 +5026,19 @@
     </row>
     <row r="33" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="C33" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="D33" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="E33" s="22" t="s">
         <v>298</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>299</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -5063,19 +5063,19 @@
     </row>
     <row r="34" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="C34" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="D34" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="E34" s="22" t="s">
         <v>303</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>304</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="11"/>
@@ -5100,19 +5100,19 @@
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="C35" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="D35" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="E35" s="22" t="s">
         <v>308</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>309</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -5133,13 +5133,13 @@
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="C36" s="15" t="s">
         <v>311</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>312</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -5162,19 +5162,19 @@
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="C37" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>315</v>
-      </c>
       <c r="D37" s="22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
@@ -5195,19 +5195,19 @@
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="C38" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="D38" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="E38" s="22" t="s">
         <v>319</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>320</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -5228,16 +5228,16 @@
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="C39" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="C39" s="15" t="s">
-        <v>323</v>
-      </c>
       <c r="D39" s="22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="11"/>
@@ -5259,16 +5259,16 @@
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="D40" s="22" t="s">
         <v>325</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>326</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="11"/>
@@ -5290,17 +5290,17 @@
     </row>
     <row r="41" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="C41" s="15" t="s">
         <v>328</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>329</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -5321,22 +5321,22 @@
     </row>
     <row r="42" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="C42" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="C42" s="15" t="s">
-        <v>332</v>
-      </c>
       <c r="D42" s="22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G42" s="11"/>
       <c r="J42" s="11"/>
@@ -5356,19 +5356,19 @@
     </row>
     <row r="43" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="C43" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="D43" s="22" t="s">
         <v>335</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="E43" s="22" t="s">
         <v>336</v>
-      </c>
-      <c r="E43" s="22" t="s">
-        <v>337</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -5389,16 +5389,16 @@
     </row>
     <row r="44" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="C44" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>340</v>
-      </c>
       <c r="D44" s="22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="11"/>
@@ -5420,28 +5420,28 @@
     </row>
     <row r="45" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="C45" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="D45" s="22" t="s">
         <v>343</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="E45" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="F45" s="6" t="s">
         <v>345</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>346</v>
       </c>
       <c r="G45" s="11"/>
       <c r="J45" s="11"/>
       <c r="K45" s="10"/>
       <c r="L45" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M45" s="11"/>
       <c r="O45" s="11"/>
@@ -5459,16 +5459,16 @@
     </row>
     <row r="46" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="C46" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="D46" s="22" t="s">
         <v>350</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>351</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="11"/>
@@ -5490,19 +5490,19 @@
     </row>
     <row r="47" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="C47" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="D47" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="E47" s="22" t="s">
         <v>354</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>354</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>355</v>
       </c>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -5523,19 +5523,19 @@
     </row>
     <row r="48" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="C48" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="D48" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="E48" s="23" t="s">
         <v>358</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="E48" s="23" t="s">
-        <v>359</v>
       </c>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
@@ -5556,16 +5556,16 @@
     </row>
     <row r="49" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="C49" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="D49" s="22" t="s">
         <v>361</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>362</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="11"/>
@@ -5587,19 +5587,19 @@
     </row>
     <row r="50" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="C50" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="D50" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="E50" s="22" t="s">
         <v>365</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>365</v>
-      </c>
-      <c r="E50" s="22" t="s">
-        <v>366</v>
       </c>
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
@@ -5620,19 +5620,19 @@
     </row>
     <row r="51" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="C51" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="D51" s="22" t="s">
+        <v>368</v>
+      </c>
+      <c r="E51" s="22" t="s">
         <v>369</v>
-      </c>
-      <c r="D51" s="22" t="s">
-        <v>369</v>
-      </c>
-      <c r="E51" s="22" t="s">
-        <v>370</v>
       </c>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
@@ -5653,17 +5653,17 @@
     </row>
     <row r="52" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B52" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="C52" s="15" t="s">
         <v>372</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>373</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
@@ -5684,26 +5684,26 @@
     </row>
     <row r="53" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="C53" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="D53" s="22" t="s">
         <v>376</v>
       </c>
-      <c r="D53" s="22" t="s">
-        <v>377</v>
-      </c>
       <c r="E53" s="22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="J53" s="11"/>
       <c r="K53" s="10"/>
       <c r="L53" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M53" s="11"/>
       <c r="O53" s="11"/>
@@ -5721,16 +5721,16 @@
     </row>
     <row r="54" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="C54" s="15" t="s">
         <v>380</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="D54" s="22" t="s">
         <v>381</v>
-      </c>
-      <c r="D54" s="22" t="s">
-        <v>382</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="11"/>
@@ -5738,7 +5738,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="10"/>
       <c r="L54" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M54" s="11"/>
       <c r="O54" s="11"/>
@@ -5756,19 +5756,19 @@
     </row>
     <row r="55" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="C55" s="15" t="s">
         <v>385</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="D55" s="22" t="s">
+        <v>385</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>386</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>386</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>387</v>
       </c>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
@@ -5789,13 +5789,13 @@
     </row>
     <row r="56" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B56" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="C56" s="15" t="s">
         <v>388</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>389</v>
       </c>
       <c r="D56" s="22"/>
       <c r="E56" s="22"/>
@@ -5807,7 +5807,7 @@
       <c r="P56" s="10"/>
       <c r="Q56" s="10"/>
       <c r="R56" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="S56" s="11"/>
       <c r="T56" s="11"/>
@@ -5816,7 +5816,7 @@
       <c r="W56" s="6"/>
       <c r="X56" s="6"/>
       <c r="Y56" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Z56" s="11"/>
       <c r="AA56" s="11"/>
@@ -5824,16 +5824,16 @@
     </row>
     <row r="57" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="C57" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="C57" s="15" t="s">
-        <v>392</v>
-      </c>
       <c r="D57" s="22" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E57" s="22"/>
       <c r="F57" s="11"/>
@@ -5855,25 +5855,25 @@
     </row>
     <row r="58" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="C58" s="15" t="s">
         <v>394</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="D58" s="22" t="s">
+        <v>394</v>
+      </c>
+      <c r="E58" s="22" t="s">
         <v>395</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>395</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>396</v>
       </c>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
       <c r="J58" s="11"/>
       <c r="K58" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M58" s="11"/>
       <c r="O58" s="11"/>
@@ -5891,16 +5891,16 @@
     </row>
     <row r="59" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="C59" s="15" t="s">
         <v>399</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="D59" s="22" t="s">
         <v>400</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>401</v>
       </c>
       <c r="E59" s="22"/>
       <c r="F59" s="11"/>
@@ -5917,23 +5917,23 @@
       <c r="X59" s="11"/>
       <c r="Y59" s="11"/>
       <c r="Z59" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AA59" s="11"/>
       <c r="AB59" s="11"/>
     </row>
     <row r="60" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="C60" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="C60" s="15" t="s">
-        <v>405</v>
-      </c>
       <c r="D60" s="22" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E60" s="22"/>
       <c r="F60" s="11"/>
@@ -5955,16 +5955,16 @@
     </row>
     <row r="61" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="C61" s="15" t="s">
         <v>407</v>
       </c>
-      <c r="C61" s="15" t="s">
-        <v>408</v>
-      </c>
       <c r="D61" s="22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E61" s="22"/>
       <c r="F61" s="11"/>
@@ -5986,16 +5986,16 @@
     </row>
     <row r="62" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="C62" s="15" t="s">
         <v>410</v>
       </c>
-      <c r="C62" s="15" t="s">
-        <v>411</v>
-      </c>
       <c r="D62" s="22" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E62" s="22"/>
       <c r="F62" s="11"/>
@@ -6017,16 +6017,16 @@
     </row>
     <row r="63" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="C63" s="15" t="s">
         <v>413</v>
       </c>
-      <c r="C63" s="15" t="s">
-        <v>414</v>
-      </c>
       <c r="D63" s="22" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E63" s="22"/>
       <c r="F63" s="11"/>
@@ -6048,13 +6048,13 @@
     </row>
     <row r="64" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="B64" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="C64" s="15" t="s">
         <v>416</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>417</v>
       </c>
       <c r="D64" s="22"/>
       <c r="E64" s="22"/>
@@ -6062,10 +6062,10 @@
       <c r="G64" s="11"/>
       <c r="J64" s="11"/>
       <c r="M64" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="O64" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="R64" s="11"/>
       <c r="S64" s="11"/>
@@ -6081,16 +6081,16 @@
     </row>
     <row r="65" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="C65" s="15" t="s">
         <v>418</v>
       </c>
-      <c r="C65" s="15" t="s">
-        <v>419</v>
-      </c>
       <c r="D65" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E65" s="22"/>
       <c r="F65" s="11"/>
@@ -6098,7 +6098,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="10"/>
       <c r="L65" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="M65" s="11"/>
       <c r="O65" s="11"/>
@@ -6116,16 +6116,16 @@
     </row>
     <row r="66" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E66" s="22"/>
       <c r="F66" s="11"/>
@@ -6147,26 +6147,26 @@
     </row>
     <row r="67" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="B67" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="C67" s="15" t="s">
         <v>423</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>424</v>
       </c>
       <c r="D67" s="22"/>
       <c r="E67" s="22" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G67" s="11"/>
       <c r="J67" s="11"/>
       <c r="K67" s="10"/>
       <c r="L67" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M67" s="11"/>
       <c r="O67" s="11"/>
@@ -6184,17 +6184,17 @@
     </row>
     <row r="68" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="B68" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="C68" s="15" t="s">
         <v>428</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>429</v>
       </c>
       <c r="D68" s="22"/>
       <c r="E68" s="22" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
@@ -6215,16 +6215,16 @@
     </row>
     <row r="69" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="B69" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="C69" s="15" t="s">
         <v>432</v>
       </c>
-      <c r="C69" s="15" t="s">
-        <v>433</v>
-      </c>
       <c r="D69" s="22" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E69" s="22"/>
       <c r="F69" s="11"/>
@@ -6268,7 +6268,7 @@
     </row>
     <row r="71" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="22"/>
@@ -6292,32 +6292,32 @@
     </row>
     <row r="72" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="B72" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="C72" s="15" t="s">
         <v>436</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="D72" s="22" t="s">
         <v>437</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="E72" s="22" t="s">
         <v>438</v>
-      </c>
-      <c r="E72" s="22" t="s">
-        <v>439</v>
       </c>
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
       <c r="J72" s="11"/>
       <c r="L72" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="M72" s="11"/>
       <c r="O72" s="11"/>
       <c r="P72" s="10"/>
       <c r="Q72" s="10"/>
       <c r="R72" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="S72" s="11"/>
       <c r="T72" s="11"/>
@@ -6327,26 +6327,26 @@
       <c r="X72" s="11"/>
       <c r="Y72" s="11"/>
       <c r="Z72" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AA72" s="11"/>
       <c r="AB72" s="11"/>
     </row>
     <row r="73" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="B73" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="C73" s="15" t="s">
         <v>444</v>
       </c>
-      <c r="C73" s="15" t="s">
+      <c r="D73" s="22" t="s">
         <v>445</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="E73" s="22" t="s">
         <v>446</v>
-      </c>
-      <c r="E73" s="22" t="s">
-        <v>447</v>
       </c>
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
@@ -6367,33 +6367,33 @@
     </row>
     <row r="74" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="B74" s="7" t="s">
+      <c r="C74" s="15" t="s">
         <v>449</v>
       </c>
-      <c r="C74" s="15" t="s">
+      <c r="D74" s="22" t="s">
         <v>450</v>
-      </c>
-      <c r="D74" s="22" t="s">
-        <v>451</v>
       </c>
       <c r="E74" s="22"/>
       <c r="F74" s="11"/>
       <c r="G74" s="11"/>
       <c r="J74" s="11"/>
       <c r="L74" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="M74" s="11"/>
       <c r="O74" s="11"/>
       <c r="P74" s="10"/>
       <c r="Q74" s="10"/>
       <c r="R74" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="S74" s="6" t="s">
         <v>453</v>
-      </c>
-      <c r="S74" s="6" t="s">
-        <v>454</v>
       </c>
       <c r="T74" s="11"/>
       <c r="U74" s="11"/>
@@ -6408,14 +6408,14 @@
     <row r="75" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="11"/>
       <c r="B75" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C75" s="15" t="s">
         <v>455</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>456</v>
       </c>
       <c r="D75" s="22"/>
       <c r="E75" s="22" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F75" s="11"/>
       <c r="G75" s="11"/>
@@ -6436,34 +6436,34 @@
     </row>
     <row r="76" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="B76" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="C76" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="C76" s="15" t="s">
+      <c r="D76" s="22" t="s">
         <v>460</v>
       </c>
-      <c r="D76" s="22" t="s">
+      <c r="E76" s="22" t="s">
         <v>461</v>
-      </c>
-      <c r="E76" s="22" t="s">
-        <v>462</v>
       </c>
       <c r="F76" s="11"/>
       <c r="G76" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J76" s="11"/>
       <c r="L76" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="M76" s="11"/>
       <c r="O76" s="11"/>
       <c r="P76" s="10"/>
       <c r="Q76" s="10"/>
       <c r="R76" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="S76" s="11"/>
       <c r="T76" s="11"/>
@@ -6478,19 +6478,19 @@
     </row>
     <row r="77" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="C77" s="15" t="s">
         <v>467</v>
       </c>
-      <c r="C77" s="15" t="s">
+      <c r="D77" s="22" t="s">
         <v>468</v>
       </c>
-      <c r="D77" s="22" t="s">
+      <c r="E77" s="22" t="s">
         <v>469</v>
-      </c>
-      <c r="E77" s="22" t="s">
-        <v>470</v>
       </c>
       <c r="F77" s="11"/>
       <c r="G77" s="11"/>
@@ -6511,19 +6511,19 @@
     </row>
     <row r="78" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="B78" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="C78" s="15" t="s">
         <v>472</v>
       </c>
-      <c r="C78" s="15" t="s">
+      <c r="D78" s="22" t="s">
         <v>473</v>
       </c>
-      <c r="D78" s="22" t="s">
+      <c r="E78" s="22" t="s">
         <v>474</v>
-      </c>
-      <c r="E78" s="22" t="s">
-        <v>475</v>
       </c>
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
@@ -6545,26 +6545,26 @@
     <row r="79" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="11"/>
       <c r="B79" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="C79" s="15" t="s">
         <v>476</v>
       </c>
-      <c r="C79" s="15" t="s">
+      <c r="D79" s="22" t="s">
         <v>477</v>
-      </c>
-      <c r="D79" s="22" t="s">
-        <v>478</v>
       </c>
       <c r="E79" s="22"/>
       <c r="F79" s="11"/>
       <c r="G79" s="11"/>
       <c r="H79" s="19" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J79" s="11"/>
       <c r="L79" s="10" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M79" s="11"/>
       <c r="O79" s="11"/>
@@ -6577,42 +6577,42 @@
       <c r="X79" s="11"/>
       <c r="Y79" s="11"/>
       <c r="Z79" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AA79" s="11"/>
       <c r="AB79" s="11"/>
     </row>
     <row r="80" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="B80" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="C80" s="15" t="s">
         <v>482</v>
       </c>
-      <c r="C80" s="15" t="s">
+      <c r="D80" s="24" t="s">
         <v>483</v>
       </c>
-      <c r="D80" s="24" t="s">
-        <v>484</v>
-      </c>
       <c r="E80" s="22" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G80" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="H80" s="11" t="s">
         <v>624</v>
-      </c>
-      <c r="H80" s="11" t="s">
-        <v>625</v>
       </c>
       <c r="J80" s="11"/>
       <c r="M80" s="6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="O80" s="6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="R80" s="11"/>
       <c r="S80" s="11"/>
@@ -6623,26 +6623,26 @@
       <c r="X80" s="11"/>
       <c r="Y80" s="11"/>
       <c r="Z80" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="AA80" s="11"/>
       <c r="AB80" s="11"/>
     </row>
     <row r="81" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B81" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="C81" s="15" t="s">
         <v>487</v>
       </c>
-      <c r="C81" s="15" t="s">
+      <c r="D81" s="22" t="s">
         <v>488</v>
       </c>
-      <c r="D81" s="22" t="s">
+      <c r="E81" s="22" t="s">
         <v>489</v>
-      </c>
-      <c r="E81" s="22" t="s">
-        <v>490</v>
       </c>
       <c r="F81" s="11"/>
       <c r="G81" s="11"/>
@@ -6663,33 +6663,33 @@
     </row>
     <row r="82" spans="1:28" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="B82" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="B82" s="7" t="s">
+      <c r="C82" s="15" t="s">
         <v>492</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="D82" s="22" t="s">
         <v>493</v>
       </c>
-      <c r="D82" s="22" t="s">
+      <c r="E82" s="22" t="s">
         <v>494</v>
-      </c>
-      <c r="E82" s="22" t="s">
-        <v>495</v>
       </c>
       <c r="F82" s="11"/>
       <c r="G82" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J82" s="11"/>
       <c r="M82" s="11"/>
       <c r="O82" s="11"/>
       <c r="P82" s="10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q82" s="10"/>
       <c r="R82" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="S82" s="11"/>
       <c r="T82" s="11"/>
@@ -6704,29 +6704,29 @@
     </row>
     <row r="83" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="B83" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="C83" s="15" t="s">
         <v>499</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>500</v>
       </c>
       <c r="D83" s="22"/>
       <c r="E83" s="22" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F83" s="11"/>
       <c r="G83" s="11"/>
       <c r="J83" s="11"/>
       <c r="L83" s="17" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M83" s="11"/>
       <c r="O83" s="11"/>
       <c r="Q83" s="10"/>
       <c r="R83" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="S83" s="11"/>
       <c r="T83" s="11"/>
@@ -6736,28 +6736,28 @@
       <c r="X83" s="11"/>
       <c r="Y83" s="11"/>
       <c r="Z83" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="AA83" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="AB83" s="11"/>
     </row>
     <row r="84" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="B84" s="7" t="s">
         <v>505</v>
       </c>
-      <c r="B84" s="7" t="s">
+      <c r="C84" s="15" t="s">
         <v>506</v>
       </c>
-      <c r="C84" s="15" t="s">
+      <c r="D84" s="22" t="s">
         <v>507</v>
       </c>
-      <c r="D84" s="22" t="s">
+      <c r="E84" s="22" t="s">
         <v>508</v>
-      </c>
-      <c r="E84" s="22" t="s">
-        <v>509</v>
       </c>
       <c r="F84" s="11"/>
       <c r="G84" s="11"/>
@@ -6765,10 +6765,10 @@
       <c r="M84" s="11"/>
       <c r="O84" s="11"/>
       <c r="Q84" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="R84" s="6" t="s">
         <v>510</v>
-      </c>
-      <c r="R84" s="6" t="s">
-        <v>511</v>
       </c>
       <c r="S84" s="11"/>
       <c r="T84" s="11"/>
@@ -6776,7 +6776,7 @@
       <c r="V84" s="11"/>
       <c r="W84" s="6"/>
       <c r="X84" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="Y84" s="11"/>
       <c r="Z84" s="11"/>
@@ -6785,16 +6785,16 @@
     </row>
     <row r="85" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="B85" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="C85" s="15" t="s">
         <v>514</v>
       </c>
-      <c r="C85" s="15" t="s">
+      <c r="D85" s="22" t="s">
         <v>515</v>
-      </c>
-      <c r="D85" s="22" t="s">
-        <v>516</v>
       </c>
       <c r="E85" s="22"/>
       <c r="F85" s="11"/>
@@ -6803,7 +6803,7 @@
       <c r="M85" s="11"/>
       <c r="O85" s="11"/>
       <c r="R85" s="6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="S85" s="11"/>
       <c r="T85" s="11"/>
@@ -6818,22 +6818,22 @@
     </row>
     <row r="86" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="B86" s="7" t="s">
         <v>518</v>
       </c>
-      <c r="B86" s="7" t="s">
+      <c r="C86" s="15" t="s">
         <v>519</v>
       </c>
-      <c r="C86" s="15" t="s">
-        <v>520</v>
-      </c>
       <c r="D86" s="22" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E86" s="22"/>
       <c r="F86" s="11"/>
       <c r="G86" s="11"/>
       <c r="I86" s="19" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J86" s="11"/>
       <c r="M86" s="11"/>
@@ -6852,16 +6852,16 @@
     </row>
     <row r="87" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>521</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="C87" s="15" t="s">
         <v>522</v>
       </c>
-      <c r="C87" s="15" t="s">
+      <c r="D87" s="22" t="s">
         <v>523</v>
-      </c>
-      <c r="D87" s="22" t="s">
-        <v>524</v>
       </c>
       <c r="E87" s="22"/>
       <c r="F87" s="11"/>
@@ -6875,7 +6875,7 @@
       <c r="U87" s="11"/>
       <c r="V87" s="11"/>
       <c r="W87" s="6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="X87" s="11"/>
       <c r="Y87" s="11"/>
@@ -6885,19 +6885,19 @@
     </row>
     <row r="88" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="B88" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="C88" s="15" t="s">
         <v>527</v>
       </c>
-      <c r="C88" s="15" t="s">
+      <c r="D88" s="22" t="s">
         <v>528</v>
       </c>
-      <c r="D88" s="22" t="s">
+      <c r="E88" s="22" t="s">
         <v>529</v>
-      </c>
-      <c r="E88" s="22" t="s">
-        <v>530</v>
       </c>
       <c r="F88" s="11"/>
       <c r="G88" s="11"/>
@@ -6910,7 +6910,7 @@
       <c r="U88" s="11"/>
       <c r="V88" s="11"/>
       <c r="W88" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="X88" s="11"/>
       <c r="Y88" s="11"/>
@@ -6920,19 +6920,19 @@
     </row>
     <row r="89" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="B89" s="7" t="s">
         <v>532</v>
       </c>
-      <c r="B89" s="7" t="s">
+      <c r="C89" s="15" t="s">
         <v>533</v>
       </c>
-      <c r="C89" s="15" t="s">
+      <c r="D89" s="22" t="s">
         <v>534</v>
       </c>
-      <c r="D89" s="22" t="s">
+      <c r="E89" s="22" t="s">
         <v>535</v>
-      </c>
-      <c r="E89" s="22" t="s">
-        <v>536</v>
       </c>
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
@@ -6940,7 +6940,7 @@
       <c r="M89" s="11"/>
       <c r="O89" s="11"/>
       <c r="R89" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="S89" s="11"/>
       <c r="T89" s="11"/>
@@ -6955,17 +6955,17 @@
     </row>
     <row r="90" spans="1:28" ht="154" x14ac:dyDescent="0.15">
       <c r="A90" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="B90" s="7" t="s">
         <v>537</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="C90" s="15" t="s">
         <v>538</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>539</v>
       </c>
       <c r="D90" s="22"/>
       <c r="E90" s="24" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
@@ -6973,7 +6973,7 @@
       <c r="M90" s="11"/>
       <c r="O90" s="11"/>
       <c r="R90" s="6" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="S90" s="11"/>
       <c r="T90" s="11"/>
@@ -6983,29 +6983,29 @@
       <c r="X90" s="11"/>
       <c r="Y90" s="11"/>
       <c r="Z90" s="11" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="AA90" s="11"/>
       <c r="AB90" s="11"/>
     </row>
     <row r="91" spans="1:28" ht="84" x14ac:dyDescent="0.15">
       <c r="A91" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="B91" s="7" t="s">
         <v>542</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="C91" s="15" t="s">
         <v>543</v>
       </c>
-      <c r="C91" s="15" t="s">
+      <c r="D91" s="22" t="s">
         <v>544</v>
-      </c>
-      <c r="D91" s="22" t="s">
-        <v>545</v>
       </c>
       <c r="E91" s="22"/>
       <c r="F91" s="11"/>
       <c r="G91" s="11"/>
       <c r="I91" s="11" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J91" s="11"/>
       <c r="M91" s="11"/>
@@ -7024,13 +7024,13 @@
     </row>
     <row r="92" spans="1:28" ht="126" x14ac:dyDescent="0.15">
       <c r="A92" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B92" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="C92" s="15" t="s">
         <v>546</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>547</v>
       </c>
       <c r="D92" s="22"/>
       <c r="E92" s="22"/>
@@ -7040,19 +7040,19 @@
       <c r="M92" s="11"/>
       <c r="O92" s="11"/>
       <c r="R92" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="S92" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="T92" s="11"/>
       <c r="U92" s="11"/>
       <c r="V92" s="11"/>
       <c r="W92" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="X92" s="6" t="s">
         <v>548</v>
-      </c>
-      <c r="X92" s="6" t="s">
-        <v>549</v>
       </c>
       <c r="Y92" s="11"/>
       <c r="Z92" s="11"/>
@@ -7061,19 +7061,19 @@
     </row>
     <row r="93" spans="1:28" ht="70" x14ac:dyDescent="0.15">
       <c r="A93" s="6" t="s">
+        <v>549</v>
+      </c>
+      <c r="B93" s="7" t="s">
         <v>550</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="C93" s="15" t="s">
         <v>551</v>
       </c>
-      <c r="C93" s="15" t="s">
+      <c r="D93" s="22" t="s">
         <v>552</v>
       </c>
-      <c r="D93" s="22" t="s">
+      <c r="E93" s="22" t="s">
         <v>553</v>
-      </c>
-      <c r="E93" s="22" t="s">
-        <v>554</v>
       </c>
       <c r="F93" s="11"/>
       <c r="G93" s="11"/>
@@ -7094,19 +7094,19 @@
     </row>
     <row r="94" spans="1:28" ht="70" x14ac:dyDescent="0.15">
       <c r="A94" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B94" s="7" t="s">
         <v>555</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="C94" s="15" t="s">
         <v>556</v>
       </c>
-      <c r="C94" s="15" t="s">
+      <c r="D94" s="22" t="s">
         <v>557</v>
       </c>
-      <c r="D94" s="22" t="s">
+      <c r="E94" s="22" t="s">
         <v>558</v>
-      </c>
-      <c r="E94" s="22" t="s">
-        <v>559</v>
       </c>
       <c r="F94" s="11"/>
       <c r="G94" s="11"/>
@@ -7114,7 +7114,7 @@
       <c r="M94" s="11"/>
       <c r="O94" s="11"/>
       <c r="R94" s="6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="S94" s="11"/>
       <c r="T94" s="11"/>
@@ -7122,7 +7122,7 @@
       <c r="V94" s="11"/>
       <c r="W94" s="11"/>
       <c r="X94" s="6" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="Y94" s="11"/>
       <c r="Z94" s="11"/>
@@ -7131,27 +7131,27 @@
     </row>
     <row r="95" spans="1:28" ht="70" x14ac:dyDescent="0.15">
       <c r="A95" s="6" t="s">
+        <v>561</v>
+      </c>
+      <c r="B95" s="7" t="s">
         <v>562</v>
       </c>
-      <c r="B95" s="7" t="s">
+      <c r="C95" s="15" t="s">
         <v>563</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>564</v>
       </c>
       <c r="D95" s="22"/>
       <c r="E95" s="22" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F95" s="11"/>
       <c r="G95" s="6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J95" s="11"/>
       <c r="M95" s="11"/>
       <c r="O95" s="11"/>
       <c r="R95" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S95" s="11"/>
       <c r="T95" s="11"/>
@@ -7161,23 +7161,23 @@
       <c r="X95" s="11"/>
       <c r="Y95" s="11"/>
       <c r="Z95" s="11" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="AA95" s="11"/>
       <c r="AB95" s="11"/>
     </row>
     <row r="96" spans="1:28" ht="98" x14ac:dyDescent="0.15">
       <c r="A96" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="B96" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="B96" s="7" t="s">
+      <c r="C96" s="15" t="s">
         <v>568</v>
       </c>
-      <c r="C96" s="15" t="s">
+      <c r="D96" s="22" t="s">
         <v>569</v>
-      </c>
-      <c r="D96" s="22" t="s">
-        <v>570</v>
       </c>
       <c r="E96" s="22"/>
       <c r="F96" s="11"/>
@@ -7187,14 +7187,14 @@
       <c r="O96" s="11"/>
       <c r="R96" s="11"/>
       <c r="S96" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="T96" s="11"/>
       <c r="U96" s="11"/>
       <c r="V96" s="11"/>
       <c r="W96" s="11"/>
       <c r="X96" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="Y96" s="11"/>
       <c r="Z96" s="11"/>
@@ -7203,44 +7203,44 @@
     </row>
     <row r="97" spans="1:28" ht="112" x14ac:dyDescent="0.15">
       <c r="A97" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="B97" s="7" t="s">
         <v>573</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="C97" s="15" t="s">
         <v>574</v>
       </c>
-      <c r="C97" s="15" t="s">
+      <c r="D97" s="22" t="s">
         <v>575</v>
       </c>
-      <c r="D97" s="22" t="s">
+      <c r="E97" s="22" t="s">
         <v>576</v>
-      </c>
-      <c r="E97" s="22" t="s">
-        <v>577</v>
       </c>
       <c r="F97" s="11"/>
       <c r="G97" s="11"/>
       <c r="J97" s="11"/>
       <c r="M97" s="6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="N97" s="10" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O97" s="6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="R97" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="S97" s="11"/>
       <c r="T97" s="11"/>
       <c r="U97" s="11"/>
       <c r="V97" s="11" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="W97" s="11"/>
       <c r="X97" s="6" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Y97" s="11"/>
       <c r="Z97" s="11"/>
@@ -7250,29 +7250,29 @@
     <row r="98" spans="1:28" ht="70" x14ac:dyDescent="0.15">
       <c r="A98" s="11"/>
       <c r="B98" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="C98" s="15" t="s">
         <v>579</v>
-      </c>
-      <c r="C98" s="15" t="s">
-        <v>580</v>
       </c>
       <c r="D98" s="22"/>
       <c r="E98" s="23" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J98" s="11"/>
       <c r="M98" s="11"/>
       <c r="O98" s="11"/>
       <c r="R98" s="6" t="s">
+        <v>581</v>
+      </c>
+      <c r="S98" s="6" t="s">
         <v>582</v>
-      </c>
-      <c r="S98" s="6" t="s">
-        <v>583</v>
       </c>
       <c r="T98" s="11"/>
       <c r="U98" s="11"/>
@@ -7287,36 +7287,36 @@
     <row r="99" spans="1:28" ht="126" x14ac:dyDescent="0.15">
       <c r="A99" s="11"/>
       <c r="B99" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="C99" s="8" t="s">
         <v>584</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="D99" s="22" t="s">
         <v>585</v>
       </c>
-      <c r="D99" s="22" t="s">
+      <c r="E99" s="22" t="s">
         <v>586</v>
-      </c>
-      <c r="E99" s="22" t="s">
-        <v>587</v>
       </c>
       <c r="F99" s="11"/>
       <c r="G99" s="11"/>
       <c r="J99" s="11"/>
       <c r="K99" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="L99" s="10" t="s">
         <v>588</v>
-      </c>
-      <c r="L99" s="10" t="s">
-        <v>589</v>
       </c>
       <c r="M99" s="11"/>
       <c r="O99" s="11"/>
       <c r="R99" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="S99" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="T99" s="14" t="s">
         <v>590</v>
-      </c>
-      <c r="S99" s="6" t="s">
-        <v>590</v>
-      </c>
-      <c r="T99" s="14" t="s">
-        <v>591</v>
       </c>
       <c r="U99" s="11"/>
       <c r="V99" s="11"/>
@@ -7330,46 +7330,46 @@
     <row r="100" spans="1:28" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A100" s="11"/>
       <c r="B100" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="C100" s="8" t="s">
         <v>592</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="D100" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="D100" s="22" t="s">
-        <v>594</v>
-      </c>
       <c r="E100" s="22" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F100" s="11"/>
       <c r="G100" s="6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H100" s="11" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I100" s="11" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J100" s="11"/>
       <c r="K100" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="L100" s="10" t="s">
         <v>595</v>
-      </c>
-      <c r="L100" s="10" t="s">
-        <v>596</v>
       </c>
       <c r="M100" s="11"/>
       <c r="O100" s="11"/>
       <c r="R100" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="S100" s="11"/>
       <c r="T100" s="14" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="U100" s="11"/>
       <c r="V100" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W100" s="11"/>
       <c r="X100" s="11"/>
@@ -7377,41 +7377,41 @@
       <c r="Z100" s="11"/>
       <c r="AA100" s="11"/>
       <c r="AB100" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="101" spans="1:28" ht="154" x14ac:dyDescent="0.15">
       <c r="A101" s="11"/>
       <c r="B101" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="C101" s="15" t="s">
         <v>600</v>
       </c>
-      <c r="C101" s="15" t="s">
+      <c r="D101" s="22" t="s">
         <v>601</v>
       </c>
-      <c r="D101" s="22" t="s">
+      <c r="E101" s="22" t="s">
         <v>602</v>
-      </c>
-      <c r="E101" s="22" t="s">
-        <v>603</v>
       </c>
       <c r="F101" s="11"/>
       <c r="G101" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="H101" s="11" t="s">
+        <v>634</v>
+      </c>
+      <c r="I101" s="10" t="s">
         <v>636</v>
-      </c>
-      <c r="H101" s="11" t="s">
-        <v>635</v>
-      </c>
-      <c r="I101" s="10" t="s">
-        <v>637</v>
       </c>
       <c r="J101" s="11"/>
       <c r="L101" s="10" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="M101" s="11"/>
       <c r="O101" s="11"/>
       <c r="R101" s="6" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="S101" s="11"/>
       <c r="T101" s="11"/>
@@ -7420,7 +7420,7 @@
       <c r="W101" s="11"/>
       <c r="X101" s="11"/>
       <c r="Y101" s="6" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="Z101" s="11"/>
       <c r="AA101" s="11"/>
@@ -7429,16 +7429,16 @@
     <row r="102" spans="1:28" ht="70" x14ac:dyDescent="0.15">
       <c r="A102" s="11"/>
       <c r="B102" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="C102" s="15" t="s">
         <v>607</v>
       </c>
-      <c r="C102" s="15" t="s">
+      <c r="D102" s="22" t="s">
         <v>608</v>
       </c>
-      <c r="D102" s="22" t="s">
+      <c r="E102" s="22" t="s">
         <v>609</v>
-      </c>
-      <c r="E102" s="22" t="s">
-        <v>610</v>
       </c>
       <c r="F102" s="11"/>
       <c r="G102" s="11"/>
@@ -7446,10 +7446,10 @@
       <c r="M102" s="11"/>
       <c r="O102" s="11"/>
       <c r="R102" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="S102" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="T102" s="11"/>
       <c r="U102" s="11"/>
@@ -7464,33 +7464,33 @@
     <row r="103" spans="1:28" ht="84" x14ac:dyDescent="0.15">
       <c r="A103" s="11"/>
       <c r="B103" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="C103" s="15" t="s">
         <v>612</v>
       </c>
-      <c r="C103" s="15" t="s">
-        <v>613</v>
-      </c>
       <c r="D103" s="22" t="s">
+        <v>637</v>
+      </c>
+      <c r="E103" s="22" t="s">
         <v>638</v>
-      </c>
-      <c r="E103" s="22" t="s">
-        <v>639</v>
       </c>
       <c r="F103" s="11"/>
       <c r="G103" s="6" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J103" s="11"/>
       <c r="M103" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="N103" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="O103" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="R103" s="11"/>
       <c r="S103" s="11"/>
@@ -7506,24 +7506,24 @@
     </row>
     <row r="104" spans="1:28" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A104" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="B104" s="7" t="s">
         <v>614</v>
       </c>
-      <c r="B104" s="7" t="s">
+      <c r="C104" s="8" t="s">
         <v>615</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>616</v>
       </c>
       <c r="D104" s="22"/>
       <c r="E104" s="22" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F104" s="11"/>
       <c r="G104" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="H104" s="11" t="s">
         <v>642</v>
-      </c>
-      <c r="H104" s="11" t="s">
-        <v>643</v>
       </c>
       <c r="J104" s="11"/>
       <c r="M104" s="11"/>
@@ -7531,11 +7531,11 @@
       <c r="R104" s="11"/>
       <c r="S104" s="11"/>
       <c r="T104" s="11" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="U104" s="11"/>
       <c r="V104" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="W104" s="11"/>
       <c r="X104" s="11"/>
@@ -7543,36 +7543,36 @@
       <c r="Z104" s="11"/>
       <c r="AA104" s="11"/>
       <c r="AB104" s="6" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="105" spans="1:28" ht="306" x14ac:dyDescent="0.15">
       <c r="A105" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B105" s="7" t="s">
         <v>618</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="C105" s="15" t="s">
         <v>619</v>
       </c>
-      <c r="C105" s="15" t="s">
+      <c r="D105" s="22" t="s">
         <v>620</v>
       </c>
-      <c r="D105" s="22" t="s">
+      <c r="E105" s="22" t="s">
         <v>621</v>
       </c>
-      <c r="E105" s="22" t="s">
+      <c r="F105" s="6" t="s">
         <v>622</v>
       </c>
-      <c r="F105" s="6" t="s">
-        <v>623</v>
-      </c>
       <c r="G105" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="H105" s="11" t="s">
         <v>646</v>
       </c>
-      <c r="H105" s="11" t="s">
+      <c r="I105" s="19" t="s">
         <v>647</v>
-      </c>
-      <c r="I105" s="19" t="s">
-        <v>648</v>
       </c>
       <c r="J105" s="11"/>
       <c r="M105" s="11"/>

</xml_diff>